<commit_message>
feat: troca de arquivos
</commit_message>
<xml_diff>
--- a/sistema.xlsx
+++ b/sistema.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -623,8 +623,10 @@
           <t>Barão de Duprat</t>
         </is>
       </c>
-      <c r="H3" t="n">
-        <v>89</v>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -641,11 +643,15 @@
           <t>SP</t>
         </is>
       </c>
-      <c r="L3" t="n">
-        <v>17998324774</v>
-      </c>
-      <c r="M3" t="n">
-        <v>738945</v>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>17998324774</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>738945</t>
+        </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -658,156 +664,6 @@
         </is>
       </c>
       <c r="P3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>usp-45030275899</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Antônio Pereira</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>03/10/2000</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>450.302.758-99</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>antoniopereira@gmail.com</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>15035-160</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Guiomar Assad Callil</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>89</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Vila Itália</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>São José do Rio Preto</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>17999234994</v>
-      </c>
-      <c r="M4" t="n">
-        <v>107593</v>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Engenharia Civil</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>usp</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>unifesp-45030298499</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Luana Rogrigues</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>13/12/2002</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>450.302.984-99</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>antoniopereira@gmail.com</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>01023-001</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Barão de Duprat</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>89</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Centro</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>São Paulo</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>17998324774</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>738945</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Engenharia Química</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>unifesp</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>